<commit_message>
Updated V4 PCB: L1 inductor from 47uF to 100uF (better low current regulation)
</commit_message>
<xml_diff>
--- a/bin/PCB/v4/BOM_TSDZ2-ESP32-v4.xlsx
+++ b/bin/PCB/v4/BOM_TSDZ2-ESP32-v4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SO000228\Desktop\TSDZ2_ESP32_v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SO000228\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5109F57-F7DF-4A6C-90E3-AE49C74EF20A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64550B13-9478-4FB1-A50C-2AC62EF8C723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="22872" windowHeight="11064" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1512" yWindow="912" windowWidth="21528" windowHeight="12048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PCB_2021-10-07" sheetId="1" r:id="rId1"/>
@@ -238,18 +238,9 @@
     <t>Sunlord</t>
   </si>
   <si>
-    <t>SWPA5040S470MT</t>
-  </si>
-  <si>
-    <t>INDUCTOR SMD 47uF 0.9A 5x5mm</t>
-  </si>
-  <si>
     <t>SMD_L5.0-W5.0</t>
   </si>
   <si>
-    <t>C86617</t>
-  </si>
-  <si>
     <t>U6,U5</t>
   </si>
   <si>
@@ -458,6 +449,15 @@
   </si>
   <si>
     <t>B-2100S06P-B110</t>
+  </si>
+  <si>
+    <t>SWPA5040S101MT</t>
+  </si>
+  <si>
+    <t>INDUCTOR SMD 100uF 0.75A 5x5mm</t>
+  </si>
+  <si>
+    <t>C88132</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1400,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1570,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -1811,19 +1811,19 @@
         <v>71</v>
       </c>
       <c r="E14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" t="s">
         <v>72</v>
       </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" t="s">
-        <v>74</v>
-      </c>
       <c r="H14" t="s">
         <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1831,28 +1831,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" t="s">
         <v>77</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
         <v>78</v>
-      </c>
-      <c r="F15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1860,28 +1860,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
         <v>83</v>
       </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>84</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>85</v>
-      </c>
-      <c r="G16" t="s">
-        <v>86</v>
-      </c>
-      <c r="H16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I16" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1889,28 +1889,28 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I17" t="s">
         <v>90</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1918,28 +1918,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" t="s">
         <v>95</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" t="s">
-        <v>97</v>
-      </c>
-      <c r="H18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1947,28 +1947,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" t="s">
         <v>100</v>
       </c>
-      <c r="E19" t="s">
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
         <v>101</v>
-      </c>
-      <c r="F19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1976,28 +1976,28 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" t="s">
         <v>106</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" t="s">
         <v>107</v>
-      </c>
-      <c r="F20" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -2005,28 +2005,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -2034,28 +2034,28 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" t="s">
         <v>116</v>
       </c>
-      <c r="E22" t="s">
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
         <v>117</v>
-      </c>
-      <c r="F22" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -2063,28 +2063,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" t="s">
         <v>77</v>
       </c>
-      <c r="E23" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" t="s">
-        <v>123</v>
-      </c>
-      <c r="G23" t="s">
-        <v>80</v>
-      </c>
       <c r="H23" t="s">
         <v>15</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -2092,28 +2092,28 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" t="s">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" t="s">
         <v>126</v>
       </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
         <v>127</v>
-      </c>
-      <c r="F24" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" t="s">
-        <v>129</v>
-      </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -2121,28 +2121,28 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" t="s">
         <v>132</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
         <v>133</v>
-      </c>
-      <c r="F25" t="s">
-        <v>134</v>
-      </c>
-      <c r="G25" t="s">
-        <v>135</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -2150,28 +2150,28 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
         <v>138</v>
-      </c>
-      <c r="E26" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>